<commit_message>
modify info table a little.
</commit_message>
<xml_diff>
--- a/Jelly_model.xlsx
+++ b/Jelly_model.xlsx
@@ -570,6 +570,7 @@
       <diagonal/>
     </border>
     <border>
+      <left/>
       <right/>
       <top/>
       <bottom/>
@@ -607,61 +608,61 @@
     </border>
   </borders>
   <cellStyleXfs count="49">
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="42" fontId="4" fillId="0" borderId="0" applyAlignment="1">
+    <xf numFmtId="42" fontId="4" fillId="0" borderId="12" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="18" borderId="0" applyAlignment="1">
+    <xf numFmtId="0" fontId="7" fillId="18" borderId="12" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="11" fillId="19" borderId="5" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="44" fontId="4" fillId="0" borderId="0" applyAlignment="1">
+    <xf numFmtId="44" fontId="4" fillId="0" borderId="12" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="41" fontId="4" fillId="0" borderId="0" applyAlignment="1">
+    <xf numFmtId="41" fontId="4" fillId="0" borderId="12" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="14" borderId="0" applyAlignment="1">
+    <xf numFmtId="0" fontId="7" fillId="14" borderId="12" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="11" borderId="0" applyAlignment="1">
+    <xf numFmtId="0" fontId="9" fillId="11" borderId="12" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="43" fontId="4" fillId="0" borderId="0" applyAlignment="1">
+    <xf numFmtId="43" fontId="4" fillId="0" borderId="12" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="24" borderId="0" applyAlignment="1">
+    <xf numFmtId="0" fontId="8" fillId="24" borderId="12" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyAlignment="1">
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="12" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="12" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyAlignment="1">
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="12" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="25" borderId="7" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="29" borderId="0" applyAlignment="1">
+    <xf numFmtId="0" fontId="8" fillId="29" borderId="12" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="12" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="12" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="12" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyAlignment="1">
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="12" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="12" fillId="0" borderId="6" applyAlignment="1">
@@ -670,13 +671,13 @@
     <xf numFmtId="0" fontId="14" fillId="0" borderId="6" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="10" borderId="0" applyAlignment="1">
+    <xf numFmtId="0" fontId="8" fillId="10" borderId="12" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="4" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="28" borderId="0" applyAlignment="1">
+    <xf numFmtId="0" fontId="8" fillId="28" borderId="12" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="18" fillId="17" borderId="8" applyAlignment="1">
@@ -688,10 +689,10 @@
     <xf numFmtId="0" fontId="20" fillId="35" borderId="9" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="23" borderId="0" applyAlignment="1">
+    <xf numFmtId="0" fontId="7" fillId="23" borderId="12" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="16" borderId="0" applyAlignment="1">
+    <xf numFmtId="0" fontId="8" fillId="16" borderId="12" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="22" fillId="0" borderId="11" applyAlignment="1">
@@ -700,58 +701,58 @@
     <xf numFmtId="0" fontId="21" fillId="0" borderId="10" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="16" fillId="27" borderId="0" applyAlignment="1">
+    <xf numFmtId="0" fontId="16" fillId="27" borderId="12" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="19" fillId="34" borderId="0" applyAlignment="1">
+    <xf numFmtId="0" fontId="19" fillId="34" borderId="12" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="22" borderId="0" applyAlignment="1">
+    <xf numFmtId="0" fontId="7" fillId="22" borderId="12" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="13" borderId="0" applyAlignment="1">
+    <xf numFmtId="0" fontId="8" fillId="13" borderId="12" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="32" borderId="0" applyAlignment="1">
+    <xf numFmtId="0" fontId="7" fillId="32" borderId="12" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="36" borderId="0" applyAlignment="1">
+    <xf numFmtId="0" fontId="7" fillId="36" borderId="12" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="31" borderId="0" applyAlignment="1">
+    <xf numFmtId="0" fontId="7" fillId="31" borderId="12" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="21" borderId="0" applyAlignment="1">
+    <xf numFmtId="0" fontId="7" fillId="21" borderId="12" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="33" borderId="0" applyAlignment="1">
+    <xf numFmtId="0" fontId="8" fillId="33" borderId="12" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="12" borderId="0" applyAlignment="1">
+    <xf numFmtId="0" fontId="8" fillId="12" borderId="12" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="9" borderId="0" applyAlignment="1">
+    <xf numFmtId="0" fontId="7" fillId="9" borderId="12" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="20" borderId="0" applyAlignment="1">
+    <xf numFmtId="0" fontId="7" fillId="20" borderId="12" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="37" borderId="0" applyAlignment="1">
+    <xf numFmtId="0" fontId="8" fillId="37" borderId="12" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="8" borderId="0" applyAlignment="1">
+    <xf numFmtId="0" fontId="7" fillId="8" borderId="12" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="15" borderId="0" applyAlignment="1">
+    <xf numFmtId="0" fontId="8" fillId="15" borderId="12" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="26" borderId="0" applyAlignment="1">
+    <xf numFmtId="0" fontId="8" fillId="26" borderId="12" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="7" borderId="0" applyAlignment="1">
+    <xf numFmtId="0" fontId="7" fillId="7" borderId="12" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="30" borderId="0" applyAlignment="1">
+    <xf numFmtId="0" fontId="8" fillId="30" borderId="12" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
@@ -11321,49 +11322,49 @@
           <t>基金</t>
         </is>
       </c>
-      <c r="E1" t="inlineStr"/>
+      <c r="E1" s="0" t="inlineStr"/>
       <c r="F1" s="0" t="inlineStr">
         <is>
           <t>基金</t>
         </is>
       </c>
-      <c r="G1" t="inlineStr"/>
+      <c r="G1" s="0" t="inlineStr"/>
       <c r="H1" s="0" t="inlineStr">
         <is>
           <t>基金</t>
         </is>
       </c>
-      <c r="I1" t="inlineStr"/>
+      <c r="I1" s="0" t="inlineStr"/>
       <c r="J1" s="0" t="inlineStr">
         <is>
           <t>基金</t>
         </is>
       </c>
-      <c r="K1" t="inlineStr"/>
+      <c r="K1" s="0" t="inlineStr"/>
       <c r="L1" s="0" t="inlineStr">
         <is>
           <t>指数</t>
         </is>
       </c>
-      <c r="M1" t="inlineStr"/>
+      <c r="M1" s="0" t="inlineStr"/>
       <c r="N1" s="0" t="inlineStr">
         <is>
           <t>指数</t>
         </is>
       </c>
-      <c r="O1" t="inlineStr"/>
+      <c r="O1" s="0" t="inlineStr"/>
       <c r="P1" s="0" t="inlineStr">
         <is>
           <t>指数</t>
         </is>
       </c>
-      <c r="Q1" t="inlineStr"/>
+      <c r="Q1" s="0" t="inlineStr"/>
       <c r="R1" s="0" t="inlineStr">
         <is>
           <t>指数</t>
         </is>
       </c>
-      <c r="S1" t="inlineStr"/>
+      <c r="S1" s="0" t="inlineStr"/>
     </row>
     <row r="2">
       <c r="A2" s="0" t="n">
@@ -11374,7 +11375,7 @@
           <t>总投资</t>
         </is>
       </c>
-      <c r="C2" t="inlineStr"/>
+      <c r="C2" s="0" t="inlineStr"/>
       <c r="D2" s="0" t="n">
         <v>501016</v>
       </c>
@@ -11388,7 +11389,7 @@
           <t>004070</t>
         </is>
       </c>
-      <c r="G2" t="inlineStr">
+      <c r="G2" s="0" t="inlineStr">
         <is>
           <t>南方中证全指证券ETF联接C</t>
         </is>
@@ -11398,7 +11399,7 @@
           <t>003096</t>
         </is>
       </c>
-      <c r="I2" t="inlineStr">
+      <c r="I2" s="0" t="inlineStr">
         <is>
           <t>中欧医疗健康混合C</t>
         </is>
@@ -11408,7 +11409,7 @@
           <t>040046</t>
         </is>
       </c>
-      <c r="K2" t="inlineStr">
+      <c r="K2" s="0" t="inlineStr">
         <is>
           <t>华安纳斯达克100指数</t>
         </is>
@@ -11458,50 +11459,50 @@
       <c r="A3" s="0" t="n">
         <v>3</v>
       </c>
-      <c r="B3" t="n">
+      <c r="B3" s="0" t="n">
         <v>64308</v>
       </c>
-      <c r="C3" t="inlineStr"/>
-      <c r="D3" t="n">
+      <c r="C3" s="0" t="inlineStr"/>
+      <c r="D3" s="0" t="n">
         <v>13000</v>
       </c>
-      <c r="E3" t="n">
+      <c r="E3" s="0" t="n">
         <v>1.0227</v>
       </c>
-      <c r="F3" t="n">
+      <c r="F3" s="0" t="n">
         <v>12000</v>
       </c>
-      <c r="G3" t="n">
+      <c r="G3" s="0" t="n">
         <v>0.9508</v>
       </c>
-      <c r="H3" t="n">
+      <c r="H3" s="0" t="n">
         <v>3000</v>
       </c>
-      <c r="I3" t="n">
+      <c r="I3" s="0" t="n">
         <v>1.764</v>
       </c>
-      <c r="J3" t="n">
+      <c r="J3" s="0" t="n">
         <v>3000</v>
       </c>
-      <c r="K3" t="n">
+      <c r="K3" s="0" t="n">
         <v>2.647</v>
       </c>
-      <c r="L3" t="n">
+      <c r="L3" s="0" t="n">
         <v>19308</v>
       </c>
-      <c r="M3" t="n">
+      <c r="M3" s="0" t="n">
         <v>27687.76</v>
       </c>
-      <c r="N3" t="n">
+      <c r="N3" s="0" t="n">
         <v>14000</v>
       </c>
-      <c r="O3" t="n">
+      <c r="O3" s="0" t="n">
         <v>4306.338</v>
       </c>
-      <c r="P3" t="inlineStr"/>
-      <c r="Q3" t="inlineStr"/>
-      <c r="R3" t="inlineStr"/>
-      <c r="S3" t="inlineStr"/>
+      <c r="P3" s="0" t="inlineStr"/>
+      <c r="Q3" s="0" t="inlineStr"/>
+      <c r="R3" s="0" t="inlineStr"/>
+      <c r="S3" s="0" t="inlineStr"/>
     </row>
     <row r="4">
       <c r="A4" s="0" t="n">
@@ -11549,10 +11550,10 @@
       <c r="O4" s="12" t="n">
         <v>2.825644699140395</v>
       </c>
-      <c r="P4" t="inlineStr"/>
-      <c r="Q4" t="inlineStr"/>
-      <c r="R4" t="inlineStr"/>
-      <c r="S4" t="inlineStr"/>
+      <c r="P4" s="0" t="inlineStr"/>
+      <c r="Q4" s="0" t="inlineStr"/>
+      <c r="R4" s="0" t="inlineStr"/>
+      <c r="S4" s="0" t="inlineStr"/>
     </row>
     <row r="5">
       <c r="A5" s="0" t="n">
@@ -11566,14 +11567,14 @@
           <t>已赎回</t>
         </is>
       </c>
-      <c r="D5" t="inlineStr"/>
-      <c r="E5" t="inlineStr"/>
-      <c r="F5" t="inlineStr"/>
-      <c r="G5" t="inlineStr"/>
-      <c r="H5" t="inlineStr"/>
-      <c r="I5" t="inlineStr"/>
-      <c r="J5" t="inlineStr"/>
-      <c r="K5" t="inlineStr"/>
+      <c r="D5" s="0" t="inlineStr"/>
+      <c r="E5" s="0" t="inlineStr"/>
+      <c r="F5" s="0" t="inlineStr"/>
+      <c r="G5" s="0" t="inlineStr"/>
+      <c r="H5" s="0" t="inlineStr"/>
+      <c r="I5" s="0" t="inlineStr"/>
+      <c r="J5" s="0" t="inlineStr"/>
+      <c r="K5" s="0" t="inlineStr"/>
       <c r="L5" s="0" t="n">
         <v>20000</v>
       </c>
@@ -11603,16 +11604,16 @@
       <c r="A6" s="0" t="n">
         <v>6</v>
       </c>
-      <c r="B6" t="inlineStr"/>
-      <c r="C6" t="inlineStr"/>
-      <c r="D6" t="inlineStr"/>
-      <c r="E6" t="inlineStr"/>
-      <c r="F6" t="inlineStr"/>
-      <c r="G6" t="inlineStr"/>
-      <c r="H6" t="inlineStr"/>
-      <c r="I6" t="inlineStr"/>
-      <c r="J6" t="inlineStr"/>
-      <c r="K6" t="inlineStr"/>
+      <c r="B6" s="0" t="inlineStr"/>
+      <c r="C6" s="0" t="inlineStr"/>
+      <c r="D6" s="0" t="inlineStr"/>
+      <c r="E6" s="0" t="inlineStr"/>
+      <c r="F6" s="0" t="inlineStr"/>
+      <c r="G6" s="0" t="inlineStr"/>
+      <c r="H6" s="0" t="inlineStr"/>
+      <c r="I6" s="0" t="inlineStr"/>
+      <c r="J6" s="0" t="inlineStr"/>
+      <c r="K6" s="0" t="inlineStr"/>
       <c r="L6" s="64" t="n">
         <v>754.844271204228</v>
       </c>
@@ -11650,14 +11651,14 @@
           <t>已赎回</t>
         </is>
       </c>
-      <c r="D7" t="inlineStr"/>
-      <c r="E7" t="inlineStr"/>
-      <c r="F7" t="inlineStr"/>
-      <c r="G7" t="inlineStr"/>
-      <c r="H7" t="inlineStr"/>
-      <c r="I7" t="inlineStr"/>
-      <c r="J7" t="inlineStr"/>
-      <c r="K7" t="inlineStr"/>
+      <c r="D7" s="0" t="inlineStr"/>
+      <c r="E7" s="0" t="inlineStr"/>
+      <c r="F7" s="0" t="inlineStr"/>
+      <c r="G7" s="0" t="inlineStr"/>
+      <c r="H7" s="0" t="inlineStr"/>
+      <c r="I7" s="0" t="inlineStr"/>
+      <c r="J7" s="0" t="inlineStr"/>
+      <c r="K7" s="0" t="inlineStr"/>
       <c r="L7" s="0" t="n">
         <v>10000</v>
       </c>
@@ -11670,25 +11671,25 @@
       <c r="O7" s="0" t="n">
         <v>4225</v>
       </c>
-      <c r="P7" t="inlineStr"/>
-      <c r="Q7" t="inlineStr"/>
-      <c r="R7" t="inlineStr"/>
-      <c r="S7" t="inlineStr"/>
+      <c r="P7" s="0" t="inlineStr"/>
+      <c r="Q7" s="0" t="inlineStr"/>
+      <c r="R7" s="0" t="inlineStr"/>
+      <c r="S7" s="0" t="inlineStr"/>
     </row>
     <row r="8">
       <c r="A8" s="0" t="n">
         <v>8</v>
       </c>
-      <c r="B8" t="inlineStr"/>
-      <c r="C8" t="inlineStr"/>
-      <c r="D8" t="inlineStr"/>
-      <c r="E8" t="inlineStr"/>
-      <c r="F8" t="inlineStr"/>
-      <c r="G8" t="inlineStr"/>
-      <c r="H8" t="inlineStr"/>
-      <c r="I8" t="inlineStr"/>
-      <c r="J8" t="inlineStr"/>
-      <c r="K8" t="inlineStr"/>
+      <c r="B8" s="0" t="inlineStr"/>
+      <c r="C8" s="0" t="inlineStr"/>
+      <c r="D8" s="0" t="inlineStr"/>
+      <c r="E8" s="0" t="inlineStr"/>
+      <c r="F8" s="0" t="inlineStr"/>
+      <c r="G8" s="0" t="inlineStr"/>
+      <c r="H8" s="0" t="inlineStr"/>
+      <c r="I8" s="0" t="inlineStr"/>
+      <c r="J8" s="0" t="inlineStr"/>
+      <c r="K8" s="0" t="inlineStr"/>
       <c r="L8" s="64" t="n">
         <v>693.237554551423</v>
       </c>
@@ -11701,10 +11702,10 @@
       <c r="O8" s="64" t="n">
         <v>1.06508875739645</v>
       </c>
-      <c r="P8" t="inlineStr"/>
-      <c r="Q8" t="inlineStr"/>
-      <c r="R8" t="inlineStr"/>
-      <c r="S8" t="inlineStr"/>
+      <c r="P8" s="0" t="inlineStr"/>
+      <c r="Q8" s="0" t="inlineStr"/>
+      <c r="R8" s="0" t="inlineStr"/>
+      <c r="S8" s="0" t="inlineStr"/>
     </row>
     <row r="9">
       <c r="A9" s="0" t="n">
@@ -11720,14 +11721,14 @@
           <t>赎回</t>
         </is>
       </c>
-      <c r="D9" t="inlineStr"/>
-      <c r="E9" t="inlineStr"/>
-      <c r="F9" t="inlineStr"/>
-      <c r="G9" t="inlineStr"/>
-      <c r="H9" t="inlineStr"/>
-      <c r="I9" t="inlineStr"/>
-      <c r="J9" t="inlineStr"/>
-      <c r="K9" t="inlineStr"/>
+      <c r="D9" s="0" t="inlineStr"/>
+      <c r="E9" s="0" t="inlineStr"/>
+      <c r="F9" s="0" t="inlineStr"/>
+      <c r="G9" s="0" t="inlineStr"/>
+      <c r="H9" s="0" t="inlineStr"/>
+      <c r="I9" s="0" t="inlineStr"/>
+      <c r="J9" s="0" t="inlineStr"/>
+      <c r="K9" s="0" t="inlineStr"/>
       <c r="L9" s="0" t="n">
         <v>-31575.22</v>
       </c>
@@ -11757,16 +11758,16 @@
       <c r="A10" s="0" t="n">
         <v>10</v>
       </c>
-      <c r="B10" t="inlineStr"/>
-      <c r="C10" t="inlineStr"/>
-      <c r="D10" t="inlineStr"/>
-      <c r="E10" t="inlineStr"/>
-      <c r="F10" t="inlineStr"/>
-      <c r="G10" t="inlineStr"/>
-      <c r="H10" t="inlineStr"/>
-      <c r="I10" t="inlineStr"/>
-      <c r="J10" t="inlineStr"/>
-      <c r="K10" t="inlineStr"/>
+      <c r="B10" s="0" t="inlineStr"/>
+      <c r="C10" s="0" t="inlineStr"/>
+      <c r="D10" s="0" t="inlineStr"/>
+      <c r="E10" s="0" t="inlineStr"/>
+      <c r="F10" s="0" t="inlineStr"/>
+      <c r="G10" s="0" t="inlineStr"/>
+      <c r="H10" s="0" t="inlineStr"/>
+      <c r="I10" s="0" t="inlineStr"/>
+      <c r="J10" s="0" t="inlineStr"/>
+      <c r="K10" s="0" t="inlineStr"/>
       <c r="L10" s="67" t="n">
         <v>1448.08</v>
       </c>
@@ -11806,14 +11807,14 @@
           <t>投资</t>
         </is>
       </c>
-      <c r="D11" t="inlineStr"/>
-      <c r="E11" t="inlineStr"/>
-      <c r="F11" t="inlineStr"/>
-      <c r="G11" t="inlineStr"/>
-      <c r="H11" t="inlineStr"/>
-      <c r="I11" t="inlineStr"/>
-      <c r="J11" t="inlineStr"/>
-      <c r="K11" t="inlineStr"/>
+      <c r="D11" s="0" t="inlineStr"/>
+      <c r="E11" s="0" t="inlineStr"/>
+      <c r="F11" s="0" t="inlineStr"/>
+      <c r="G11" s="0" t="inlineStr"/>
+      <c r="H11" s="0" t="inlineStr"/>
+      <c r="I11" s="0" t="inlineStr"/>
+      <c r="J11" s="0" t="inlineStr"/>
+      <c r="K11" s="0" t="inlineStr"/>
       <c r="L11" s="0" t="n">
         <v>14298</v>
       </c>
@@ -11826,25 +11827,25 @@
       <c r="O11" s="0" t="n">
         <v>4188</v>
       </c>
-      <c r="P11" t="inlineStr"/>
-      <c r="Q11" t="inlineStr"/>
-      <c r="R11" t="inlineStr"/>
-      <c r="S11" t="inlineStr"/>
+      <c r="P11" s="0" t="inlineStr"/>
+      <c r="Q11" s="0" t="inlineStr"/>
+      <c r="R11" s="0" t="inlineStr"/>
+      <c r="S11" s="0" t="inlineStr"/>
     </row>
     <row r="12">
       <c r="A12" s="0" t="n">
         <v>12</v>
       </c>
-      <c r="B12" t="inlineStr"/>
-      <c r="C12" t="inlineStr"/>
-      <c r="D12" t="inlineStr"/>
-      <c r="E12" t="inlineStr"/>
-      <c r="F12" t="inlineStr"/>
-      <c r="G12" t="inlineStr"/>
-      <c r="H12" t="inlineStr"/>
-      <c r="I12" t="inlineStr"/>
-      <c r="J12" t="inlineStr"/>
-      <c r="K12" t="inlineStr"/>
+      <c r="B12" s="0" t="inlineStr"/>
+      <c r="C12" s="0" t="inlineStr"/>
+      <c r="D12" s="0" t="inlineStr"/>
+      <c r="E12" s="0" t="inlineStr"/>
+      <c r="F12" s="0" t="inlineStr"/>
+      <c r="G12" s="0" t="inlineStr"/>
+      <c r="H12" s="0" t="inlineStr"/>
+      <c r="I12" s="0" t="inlineStr"/>
+      <c r="J12" s="0" t="inlineStr"/>
+      <c r="K12" s="0" t="inlineStr"/>
       <c r="L12" s="11" t="n">
         <v>539.5095566133194</v>
       </c>
@@ -11857,10 +11858,10 @@
       <c r="O12" s="11" t="n">
         <v>2.825644699140395</v>
       </c>
-      <c r="P12" t="inlineStr"/>
-      <c r="Q12" t="inlineStr"/>
-      <c r="R12" t="inlineStr"/>
-      <c r="S12" t="inlineStr"/>
+      <c r="P12" s="0" t="inlineStr"/>
+      <c r="Q12" s="0" t="inlineStr"/>
+      <c r="R12" s="0" t="inlineStr"/>
+      <c r="S12" s="0" t="inlineStr"/>
     </row>
     <row r="13">
       <c r="A13" s="0" t="n">
@@ -11879,34 +11880,34 @@
       <c r="D13" s="0" t="n">
         <v>13000</v>
       </c>
-      <c r="E13" t="n">
+      <c r="E13" s="0" t="n">
         <v>0.9656</v>
       </c>
       <c r="F13" s="0" t="n">
         <v>12000</v>
       </c>
-      <c r="G13" t="n">
+      <c r="G13" s="0" t="n">
         <v>0.8983</v>
       </c>
-      <c r="H13" t="inlineStr"/>
-      <c r="I13" t="inlineStr"/>
-      <c r="J13" t="inlineStr"/>
-      <c r="K13" t="inlineStr"/>
-      <c r="L13" t="inlineStr"/>
-      <c r="M13" t="inlineStr"/>
-      <c r="N13" t="inlineStr"/>
-      <c r="O13" t="inlineStr"/>
-      <c r="P13" t="inlineStr"/>
-      <c r="Q13" t="inlineStr"/>
-      <c r="R13" t="inlineStr"/>
-      <c r="S13" t="inlineStr"/>
+      <c r="H13" s="0" t="inlineStr"/>
+      <c r="I13" s="0" t="inlineStr"/>
+      <c r="J13" s="0" t="inlineStr"/>
+      <c r="K13" s="0" t="inlineStr"/>
+      <c r="L13" s="0" t="inlineStr"/>
+      <c r="M13" s="0" t="inlineStr"/>
+      <c r="N13" s="0" t="inlineStr"/>
+      <c r="O13" s="0" t="inlineStr"/>
+      <c r="P13" s="0" t="inlineStr"/>
+      <c r="Q13" s="0" t="inlineStr"/>
+      <c r="R13" s="0" t="inlineStr"/>
+      <c r="S13" s="0" t="inlineStr"/>
     </row>
     <row r="14">
       <c r="A14" s="0" t="n">
         <v>14</v>
       </c>
-      <c r="B14" t="inlineStr"/>
-      <c r="C14" t="inlineStr"/>
+      <c r="B14" s="0" t="inlineStr"/>
+      <c r="C14" s="0" t="inlineStr"/>
       <c r="D14" s="11" t="n">
         <v>768.7448218724099</v>
       </c>
@@ -11919,18 +11920,18 @@
       <c r="G14" s="11" t="n">
         <v>5.844372703996436</v>
       </c>
-      <c r="H14" t="inlineStr"/>
-      <c r="I14" t="inlineStr"/>
-      <c r="J14" t="inlineStr"/>
-      <c r="K14" t="inlineStr"/>
-      <c r="L14" t="inlineStr"/>
-      <c r="M14" t="inlineStr"/>
-      <c r="N14" t="inlineStr"/>
-      <c r="O14" t="inlineStr"/>
-      <c r="P14" t="inlineStr"/>
-      <c r="Q14" t="inlineStr"/>
-      <c r="R14" t="inlineStr"/>
-      <c r="S14" t="inlineStr"/>
+      <c r="H14" s="0" t="inlineStr"/>
+      <c r="I14" s="0" t="inlineStr"/>
+      <c r="J14" s="0" t="inlineStr"/>
+      <c r="K14" s="0" t="inlineStr"/>
+      <c r="L14" s="0" t="inlineStr"/>
+      <c r="M14" s="0" t="inlineStr"/>
+      <c r="N14" s="0" t="inlineStr"/>
+      <c r="O14" s="0" t="inlineStr"/>
+      <c r="P14" s="0" t="inlineStr"/>
+      <c r="Q14" s="0" t="inlineStr"/>
+      <c r="R14" s="0" t="inlineStr"/>
+      <c r="S14" s="0" t="inlineStr"/>
     </row>
     <row r="15">
       <c r="A15" s="0" t="n">
@@ -11946,53 +11947,53 @@
           <t>投资</t>
         </is>
       </c>
-      <c r="D15" t="inlineStr"/>
-      <c r="E15" t="inlineStr"/>
-      <c r="F15" t="inlineStr"/>
-      <c r="G15" t="inlineStr"/>
+      <c r="D15" s="0" t="inlineStr"/>
+      <c r="E15" s="0" t="inlineStr"/>
+      <c r="F15" s="0" t="inlineStr"/>
+      <c r="G15" s="0" t="inlineStr"/>
       <c r="H15" s="0" t="n">
         <v>3000</v>
       </c>
-      <c r="I15" t="n">
+      <c r="I15" s="0" t="n">
         <v>1.718</v>
       </c>
-      <c r="J15" t="inlineStr"/>
-      <c r="K15" t="inlineStr"/>
-      <c r="L15" t="inlineStr"/>
-      <c r="M15" t="inlineStr"/>
-      <c r="N15" t="inlineStr"/>
-      <c r="O15" t="inlineStr"/>
-      <c r="P15" t="inlineStr"/>
-      <c r="Q15" t="inlineStr"/>
-      <c r="R15" t="inlineStr"/>
-      <c r="S15" t="inlineStr"/>
+      <c r="J15" s="0" t="inlineStr"/>
+      <c r="K15" s="0" t="inlineStr"/>
+      <c r="L15" s="0" t="inlineStr"/>
+      <c r="M15" s="0" t="inlineStr"/>
+      <c r="N15" s="0" t="inlineStr"/>
+      <c r="O15" s="0" t="inlineStr"/>
+      <c r="P15" s="0" t="inlineStr"/>
+      <c r="Q15" s="0" t="inlineStr"/>
+      <c r="R15" s="0" t="inlineStr"/>
+      <c r="S15" s="0" t="inlineStr"/>
     </row>
     <row r="16">
       <c r="A16" s="0" t="n">
         <v>16</v>
       </c>
-      <c r="B16" t="inlineStr"/>
-      <c r="C16" t="inlineStr"/>
-      <c r="D16" t="inlineStr"/>
-      <c r="E16" t="inlineStr"/>
-      <c r="F16" t="inlineStr"/>
-      <c r="G16" t="inlineStr"/>
+      <c r="B16" s="0" t="inlineStr"/>
+      <c r="C16" s="0" t="inlineStr"/>
+      <c r="D16" s="0" t="inlineStr"/>
+      <c r="E16" s="0" t="inlineStr"/>
+      <c r="F16" s="0" t="inlineStr"/>
+      <c r="G16" s="0" t="inlineStr"/>
       <c r="H16" s="12" t="n">
         <v>80.32596041909204</v>
       </c>
       <c r="I16" s="12" t="n">
         <v>2.677532013969735</v>
       </c>
-      <c r="J16" t="inlineStr"/>
-      <c r="K16" t="inlineStr"/>
-      <c r="L16" t="inlineStr"/>
-      <c r="M16" t="inlineStr"/>
-      <c r="N16" t="inlineStr"/>
-      <c r="O16" t="inlineStr"/>
-      <c r="P16" t="inlineStr"/>
-      <c r="Q16" t="inlineStr"/>
-      <c r="R16" t="inlineStr"/>
-      <c r="S16" t="inlineStr"/>
+      <c r="J16" s="0" t="inlineStr"/>
+      <c r="K16" s="0" t="inlineStr"/>
+      <c r="L16" s="0" t="inlineStr"/>
+      <c r="M16" s="0" t="inlineStr"/>
+      <c r="N16" s="0" t="inlineStr"/>
+      <c r="O16" s="0" t="inlineStr"/>
+      <c r="P16" s="0" t="inlineStr"/>
+      <c r="Q16" s="0" t="inlineStr"/>
+      <c r="R16" s="0" t="inlineStr"/>
+      <c r="S16" s="0" t="inlineStr"/>
     </row>
     <row r="17">
       <c r="A17" s="0" t="n">
@@ -12008,16 +12009,16 @@
           <t>投资</t>
         </is>
       </c>
-      <c r="D17" t="inlineStr"/>
-      <c r="E17" t="inlineStr"/>
-      <c r="F17" t="inlineStr"/>
-      <c r="G17" t="inlineStr"/>
-      <c r="H17" t="inlineStr"/>
-      <c r="I17" t="inlineStr"/>
+      <c r="D17" s="0" t="inlineStr"/>
+      <c r="E17" s="0" t="inlineStr"/>
+      <c r="F17" s="0" t="inlineStr"/>
+      <c r="G17" s="0" t="inlineStr"/>
+      <c r="H17" s="0" t="inlineStr"/>
+      <c r="I17" s="0" t="inlineStr"/>
       <c r="J17" s="0" t="n">
         <v>3000</v>
       </c>
-      <c r="K17" t="n">
+      <c r="K17" s="0" t="n">
         <v>2.61</v>
       </c>
       <c r="L17" s="0" t="n">
@@ -12026,25 +12027,25 @@
       <c r="M17" s="0" t="n">
         <v>26217</v>
       </c>
-      <c r="N17" t="inlineStr"/>
-      <c r="O17" t="inlineStr"/>
-      <c r="P17" t="inlineStr"/>
-      <c r="Q17" t="inlineStr"/>
-      <c r="R17" t="inlineStr"/>
-      <c r="S17" t="inlineStr"/>
+      <c r="N17" s="0" t="inlineStr"/>
+      <c r="O17" s="0" t="inlineStr"/>
+      <c r="P17" s="0" t="inlineStr"/>
+      <c r="Q17" s="0" t="inlineStr"/>
+      <c r="R17" s="0" t="inlineStr"/>
+      <c r="S17" s="0" t="inlineStr"/>
     </row>
     <row r="18">
       <c r="A18" s="0" t="n">
         <v>18</v>
       </c>
-      <c r="B18" t="inlineStr"/>
-      <c r="C18" t="inlineStr"/>
-      <c r="D18" t="inlineStr"/>
-      <c r="E18" t="inlineStr"/>
-      <c r="F18" t="inlineStr"/>
-      <c r="G18" t="inlineStr"/>
-      <c r="H18" t="inlineStr"/>
-      <c r="I18" t="inlineStr"/>
+      <c r="B18" s="0" t="inlineStr"/>
+      <c r="C18" s="0" t="inlineStr"/>
+      <c r="D18" s="0" t="inlineStr"/>
+      <c r="E18" s="0" t="inlineStr"/>
+      <c r="F18" s="0" t="inlineStr"/>
+      <c r="G18" s="0" t="inlineStr"/>
+      <c r="H18" s="0" t="inlineStr"/>
+      <c r="I18" s="0" t="inlineStr"/>
       <c r="J18" s="12" t="n">
         <v>42.52873563218382</v>
       </c>
@@ -12057,33 +12058,33 @@
       <c r="M18" s="11" t="n">
         <v>5.609947743830333</v>
       </c>
-      <c r="N18" t="inlineStr"/>
-      <c r="O18" t="inlineStr"/>
-      <c r="P18" t="inlineStr"/>
-      <c r="Q18" t="inlineStr"/>
-      <c r="R18" t="inlineStr"/>
-      <c r="S18" t="inlineStr"/>
+      <c r="N18" s="0" t="inlineStr"/>
+      <c r="O18" s="0" t="inlineStr"/>
+      <c r="P18" s="0" t="inlineStr"/>
+      <c r="Q18" s="0" t="inlineStr"/>
+      <c r="R18" s="0" t="inlineStr"/>
+      <c r="S18" s="0" t="inlineStr"/>
     </row>
     <row r="19">
-      <c r="A19" t="inlineStr"/>
-      <c r="B19" t="inlineStr"/>
-      <c r="C19" t="inlineStr"/>
-      <c r="D19" t="inlineStr"/>
-      <c r="E19" t="inlineStr"/>
-      <c r="F19" t="inlineStr"/>
-      <c r="G19" t="inlineStr"/>
-      <c r="H19" t="inlineStr"/>
-      <c r="I19" t="inlineStr"/>
-      <c r="J19" t="inlineStr"/>
-      <c r="K19" t="inlineStr"/>
-      <c r="L19" t="inlineStr"/>
-      <c r="M19" t="inlineStr"/>
-      <c r="N19" t="inlineStr"/>
-      <c r="O19" t="inlineStr"/>
-      <c r="P19" t="inlineStr"/>
-      <c r="Q19" t="inlineStr"/>
-      <c r="R19" t="inlineStr"/>
-      <c r="S19" t="inlineStr"/>
+      <c r="A19" s="0" t="inlineStr"/>
+      <c r="B19" s="0" t="inlineStr"/>
+      <c r="C19" s="0" t="inlineStr"/>
+      <c r="D19" s="0" t="inlineStr"/>
+      <c r="E19" s="0" t="inlineStr"/>
+      <c r="F19" s="0" t="inlineStr"/>
+      <c r="G19" s="0" t="inlineStr"/>
+      <c r="H19" s="0" t="inlineStr"/>
+      <c r="I19" s="0" t="inlineStr"/>
+      <c r="J19" s="0" t="inlineStr"/>
+      <c r="K19" s="0" t="inlineStr"/>
+      <c r="L19" s="0" t="inlineStr"/>
+      <c r="M19" s="0" t="inlineStr"/>
+      <c r="N19" s="0" t="inlineStr"/>
+      <c r="O19" s="0" t="inlineStr"/>
+      <c r="P19" s="0" t="inlineStr"/>
+      <c r="Q19" s="0" t="inlineStr"/>
+      <c r="R19" s="0" t="inlineStr"/>
+      <c r="S19" s="0" t="inlineStr"/>
     </row>
     <row r="20"/>
     <row r="21">
@@ -12806,13 +12807,16 @@
       </c>
       <c r="G4" s="0" t="inlineStr">
         <is>
-          <t>美国认为经济好于预期，暂停降息刺激。好消息。</t>
+          <t>美国认为经济好于预期，
+暂停降息刺激。好消息。</t>
         </is>
       </c>
       <c r="H4" s="0" t="inlineStr">
         <is>
           <t>美国三次降息后暂停降息。持利率在1.50%-1.75%不变。
-美国近日公布的经济数据也为美联储近期不再进一步降息提供了支撑。GDP数据显示，美国第三季度GDP同比增长1.9%，略低于第二季度的2.0%，但强于市场预测的1.6%。</t>
+美国近日公布的经济数据也为美联储近期不再进一步降息提供了支撑。
+GDP数据显示，美国第三季度GDP同比增长1.9%，
+略低于第二季度的2.0%，但强于市场预测的1.6%。</t>
         </is>
       </c>
     </row>

</xml_diff>